<commit_message>
Nissan French portal, Prod Code upgration, xpath changes for different portals, new calculation logic code changes, reformationg result data sheet
</commit_message>
<xml_diff>
--- a/Result - Prod.xlsx
+++ b/Result - Prod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enayem\Documents\DTC_katalon - V.4.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enayem\Documents\DTC_katalon - V.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F00DE4FE-9D55-4E60-9211-1E7BB319E4D0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{99AF873D-7D9C-46D7-B292-FE481536D168}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="1" tabRatio="514" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView tabRatio="514" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Vroom_result" r:id="rId1" sheetId="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="244">
   <si>
     <t>TestCase</t>
   </si>
@@ -360,9 +360,6 @@
     <t>oneprotectdtc139817</t>
   </si>
   <si>
-    <t>24 months</t>
-  </si>
-  <si>
     <t>_hc_err is occured and _hc_lastop is not Synced. Please check</t>
   </si>
   <si>
@@ -519,266 +516,270 @@
     <t>Vroom</t>
   </si>
   <si>
-    <t>WA1VXBF70PD030251</t>
-  </si>
-  <si>
     <t>24001</t>
   </si>
   <si>
-    <t>$2,707.10</t>
-  </si>
-  <si>
     <t>10/25/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">For customized initial Pay: 10% ,Monthly payment after initial pay is : 2461.0 || For 36months Remaining payment, calculation is matched in Cart page </t>
-  </si>
-  <si>
     <t>2 YEARS, 24,000 MILES</t>
   </si>
   <si>
     <t>12 months</t>
   </si>
   <si>
-    <t>$2,461.00</t>
-  </si>
-  <si>
-    <t>$172.27</t>
-  </si>
-  <si>
-    <t>$2,633.27</t>
-  </si>
-  <si>
-    <t>c140761</t>
-  </si>
-  <si>
-    <t>Total dues after initial pay is : 2387.17 || For 36 Remaining payment calculation is matched in Checkout page</t>
-  </si>
-  <si>
     <t>nissan</t>
   </si>
   <si>
     <t>ON</t>
   </si>
   <si>
-    <t>4 year\(s\) or 60,000 kilometers</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>c140759</t>
-  </si>
-  <si>
-    <t>QC</t>
-  </si>
-  <si>
     <t>standardoilchange</t>
   </si>
   <si>
-    <t>2 year\(s\) or 48,000 kilometers</t>
+    <t>00000SC2</t>
+  </si>
+  <si>
+    <t>WBADZ4C07MCF72424</t>
+  </si>
+  <si>
+    <t>6 YEARS, 60,000 MILES</t>
+  </si>
+  <si>
+    <t>$3,511.44</t>
+  </si>
+  <si>
+    <t>oneprotectdtc140780</t>
+  </si>
+  <si>
+    <t>3GKALVEXXLL194207</t>
+  </si>
+  <si>
+    <t>$1,548.00</t>
+  </si>
+  <si>
+    <t>$100.62</t>
+  </si>
+  <si>
+    <t>1548</t>
+  </si>
+  <si>
+    <t>10/31/2023</t>
+  </si>
+  <si>
+    <t>$1,798.00</t>
+  </si>
+  <si>
+    <t>$116.87</t>
+  </si>
+  <si>
+    <t>1798</t>
+  </si>
+  <si>
+    <t>$2,148.00</t>
+  </si>
+  <si>
+    <t>$139.62</t>
+  </si>
+  <si>
+    <t>2148</t>
+  </si>
+  <si>
+    <t>$2,287.62</t>
+  </si>
+  <si>
+    <t>5GAEVAKW6KJ222068</t>
+  </si>
+  <si>
+    <t>$2,463.00</t>
+  </si>
+  <si>
+    <t>$160.10</t>
+  </si>
+  <si>
+    <t>$2,623.10</t>
+  </si>
+  <si>
+    <t>1GYS4CKL7MR210192</t>
+  </si>
+  <si>
+    <t>$2,548.00</t>
+  </si>
+  <si>
+    <t>$165.62</t>
+  </si>
+  <si>
+    <t>$2,713.62</t>
+  </si>
+  <si>
+    <t>1GNSKSKD2NR353929</t>
+  </si>
+  <si>
+    <t>$1,750.00</t>
+  </si>
+  <si>
+    <t>$113.75</t>
+  </si>
+  <si>
+    <t>$1,863.75</t>
+  </si>
+  <si>
+    <t>11/01/2023</t>
+  </si>
+  <si>
+    <t>2 YEARS, 30,000 MILES</t>
+  </si>
+  <si>
+    <t>$2,135.00</t>
+  </si>
+  <si>
+    <t>$138.78</t>
+  </si>
+  <si>
+    <t>$2,273.78</t>
+  </si>
+  <si>
+    <t>19UDE4H69PA027805</t>
+  </si>
+  <si>
+    <t>$1,998.00</t>
+  </si>
+  <si>
+    <t>$139.86</t>
+  </si>
+  <si>
+    <t>$2,137.86</t>
+  </si>
+  <si>
+    <t>11/02/2023</t>
+  </si>
+  <si>
+    <t>cartPageCalculation is not Accurate</t>
+  </si>
+  <si>
+    <t>Calculation is not matched for Checkout page</t>
+  </si>
+  <si>
+    <t>Schomp</t>
+  </si>
+  <si>
+    <t>0065500000MieFYAAZ</t>
+  </si>
+  <si>
+    <t>Emran</t>
+  </si>
+  <si>
+    <t>Nayem</t>
+  </si>
+  <si>
+    <t>36001</t>
+  </si>
+  <si>
+    <t>$6,519.76</t>
+  </si>
+  <si>
+    <t>11/08/2023</t>
+  </si>
+  <si>
+    <t>$456.38</t>
+  </si>
+  <si>
+    <t>$6,976.14</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>5 year\(s\) or 60,000 kilometers</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>$1,215.00</t>
+  </si>
+  <si>
+    <t>$157.95</t>
+  </si>
+  <si>
+    <t>$1,372.95</t>
+  </si>
+  <si>
+    <t>11/09/2023</t>
+  </si>
+  <si>
+    <t>5 year\(s\) or 120,000 kilometers</t>
+  </si>
+  <si>
+    <t>$640.00</t>
+  </si>
+  <si>
+    <t>$83.20</t>
+  </si>
+  <si>
+    <t>$723.20</t>
+  </si>
+  <si>
+    <t>0064z00002BZRmjAAH</t>
+  </si>
+  <si>
+    <t>11/15/2023</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1GNSKRKD6PR532504</t>
+  </si>
+  <si>
+    <t>$2,056.00</t>
+  </si>
+  <si>
+    <t>$133.64</t>
+  </si>
+  <si>
+    <t>$2,189.64</t>
+  </si>
+  <si>
+    <t>1GYS4BKL9PR451444</t>
+  </si>
+  <si>
+    <t>WA</t>
   </si>
   <si>
     <t>Pay In Full</t>
   </si>
   <si>
-    <t>c140768</t>
-  </si>
-  <si>
-    <t>00000SC2</t>
-  </si>
-  <si>
-    <t>WBADZ4C07MCF72424</t>
-  </si>
-  <si>
-    <t>6 YEARS, 60,000 MILES</t>
-  </si>
-  <si>
-    <t>$3,511.44</t>
-  </si>
-  <si>
-    <t>oneprotectdtc140780</t>
-  </si>
-  <si>
-    <t>3GKALVEXXLL194207</t>
-  </si>
-  <si>
-    <t>$1,548.00</t>
-  </si>
-  <si>
-    <t>$100.62</t>
-  </si>
-  <si>
-    <t>1548</t>
-  </si>
-  <si>
-    <t>10/31/2023</t>
-  </si>
-  <si>
-    <t>$1,798.00</t>
-  </si>
-  <si>
-    <t>$116.87</t>
-  </si>
-  <si>
-    <t>1798</t>
-  </si>
-  <si>
-    <t>$2,148.00</t>
-  </si>
-  <si>
-    <t>$139.62</t>
-  </si>
-  <si>
-    <t>2148</t>
-  </si>
-  <si>
-    <t>$2,287.62</t>
-  </si>
-  <si>
-    <t>5GAEVAKW6KJ222068</t>
-  </si>
-  <si>
-    <t>$2,463.00</t>
-  </si>
-  <si>
-    <t>$160.10</t>
-  </si>
-  <si>
-    <t>$2,623.10</t>
-  </si>
-  <si>
-    <t>1GYS4CKL7MR210192</t>
-  </si>
-  <si>
-    <t>$2,548.00</t>
-  </si>
-  <si>
-    <t>$165.62</t>
-  </si>
-  <si>
-    <t>$2,713.62</t>
-  </si>
-  <si>
-    <t>1GNSKSKD2NR353929</t>
-  </si>
-  <si>
-    <t>$1,750.00</t>
-  </si>
-  <si>
-    <t>$113.75</t>
-  </si>
-  <si>
-    <t>$1,863.75</t>
-  </si>
-  <si>
-    <t>11/01/2023</t>
-  </si>
-  <si>
-    <t>2 YEARS, 30,000 MILES</t>
-  </si>
-  <si>
-    <t>$2,135.00</t>
-  </si>
-  <si>
-    <t>$138.78</t>
-  </si>
-  <si>
-    <t>$2,273.78</t>
-  </si>
-  <si>
-    <t>19UDE4H69PA027805</t>
-  </si>
-  <si>
-    <t>$1,998.00</t>
-  </si>
-  <si>
-    <t>$139.86</t>
-  </si>
-  <si>
-    <t>$2,137.86</t>
-  </si>
-  <si>
-    <t>11/02/2023</t>
-  </si>
-  <si>
-    <t>cartPageCalculation is not Accurate</t>
-  </si>
-  <si>
-    <t>Calculation is not matched for Checkout page</t>
-  </si>
-  <si>
-    <t>Schomp</t>
-  </si>
-  <si>
-    <t>0065500000MieFYAAZ</t>
-  </si>
-  <si>
-    <t>Emran</t>
-  </si>
-  <si>
-    <t>Nayem</t>
-  </si>
-  <si>
-    <t>36001</t>
-  </si>
-  <si>
-    <t>$6,519.76</t>
-  </si>
-  <si>
-    <t>11/08/2023</t>
-  </si>
-  <si>
-    <t>$456.38</t>
-  </si>
-  <si>
-    <t>$6,976.14</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>5 year\(s\) or 60,000 kilometers</t>
-  </si>
-  <si>
-    <t>6 months</t>
-  </si>
-  <si>
-    <t>$1,215.00</t>
-  </si>
-  <si>
-    <t>$157.95</t>
-  </si>
-  <si>
-    <t>$1,372.95</t>
-  </si>
-  <si>
-    <t>11/09/2023</t>
-  </si>
-  <si>
-    <t>5 year\(s\) or 120,000 kilometers</t>
-  </si>
-  <si>
-    <t>$640.00</t>
-  </si>
-  <si>
-    <t>$83.20</t>
-  </si>
-  <si>
-    <t>$723.20</t>
-  </si>
-  <si>
-    <t>0064z00002BZRmjAAH</t>
+    <t>$2,822.00</t>
+  </si>
+  <si>
+    <t>$289.26</t>
+  </si>
+  <si>
+    <t>Not applicable in Pay in Full</t>
+  </si>
+  <si>
+    <t>1GKS1DKLXPR555018</t>
+  </si>
+  <si>
+    <t>$2,274.00</t>
+  </si>
+  <si>
+    <t>$147.81</t>
+  </si>
+  <si>
+    <t>LRBFZMR4XPD166346</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,13 +791,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -860,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
@@ -868,9 +862,6 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="8" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1151,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,16 +1259,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
         <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
       </c>
       <c r="F2" t="s">
         <v>67</v>
@@ -1289,22 +1280,22 @@
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>202</v>
       </c>
       <c r="M2" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
@@ -1316,10 +1307,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="S2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="Y2" t="s">
         <v>68</v>
@@ -1331,10 +1322,10 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="AD2" t="s">
-        <v>21</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -1342,16 +1333,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>154</v>
       </c>
       <c r="F3" t="s">
         <v>67</v>
@@ -1363,25 +1354,25 @@
         <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="L3" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="M3" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="N3" t="s">
         <v>56</v>
       </c>
       <c r="O3" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
         <v>21</v>
@@ -1390,7 +1381,7 @@
         <v>21</v>
       </c>
       <c r="R3" t="s">
-        <v>162</v>
+        <v>228</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
@@ -1405,84 +1396,10 @@
         <v>48</v>
       </c>
       <c r="AC3" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="AD3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" t="s">
-        <v>160</v>
-      </c>
-      <c r="J4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K4" t="s">
-        <v>216</v>
-      </c>
-      <c r="L4" t="s">
-        <v>217</v>
-      </c>
-      <c r="M4" t="s">
-        <v>218</v>
-      </c>
-      <c r="N4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R4" t="s">
-        <v>219</v>
-      </c>
-      <c r="S4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>220</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1493,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365242B-62E7-41FE-A019-18561DC38DDF}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="106" zoomScaleNormal="106">
-      <selection activeCell="A3" sqref="A3:T3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1421,7 @@
     <col min="18" max="18" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1563,270 +1480,162 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2000</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" s="4">
-        <v>780</v>
-      </c>
-      <c r="L2" s="4">
-        <v>101.4</v>
-      </c>
-      <c r="M2" s="4">
-        <v>881.4</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="5">
-        <v>45224</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>218</v>
+      </c>
+      <c r="K2" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" t="s">
+        <v>220</v>
+      </c>
+      <c r="M2" t="s">
+        <v>221</v>
+      </c>
+      <c r="N2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>222</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="I3" s="3">
-        <v>10000</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="K3" s="4">
-        <v>288</v>
-      </c>
-      <c r="L3" s="4">
-        <v>43.13</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="5">
-        <v>45224</v>
-      </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" t="s">
+        <v>217</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" t="s">
+        <v>220</v>
+      </c>
+      <c r="M3" t="s">
+        <v>221</v>
+      </c>
+      <c r="N3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" t="s">
+        <v>222</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
+        <v>165</v>
       </c>
       <c r="H4" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="I4" t="s">
         <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="K4" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="L4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="M4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="N4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4"/>
-      <c r="Q4"/>
       <c r="R4" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="S4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" t="s">
-        <v>225</v>
-      </c>
-      <c r="F5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" t="s">
-        <v>231</v>
-      </c>
-      <c r="H5" t="s">
-        <v>232</v>
-      </c>
-      <c r="I5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>233</v>
-      </c>
-      <c r="K5" t="s">
-        <v>234</v>
-      </c>
-      <c r="L5" t="s">
-        <v>235</v>
-      </c>
-      <c r="M5" t="s">
-        <v>236</v>
-      </c>
-      <c r="N5" t="s">
-        <v>174</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5" t="s">
-        <v>237</v>
-      </c>
-      <c r="S5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" t="s">
-        <v>177</v>
-      </c>
-      <c r="H6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" t="s">
-        <v>233</v>
-      </c>
-      <c r="K6" t="s">
-        <v>239</v>
-      </c>
-      <c r="L6" t="s">
-        <v>240</v>
-      </c>
-      <c r="M6" t="s">
-        <v>241</v>
-      </c>
-      <c r="N6" t="s">
-        <v>174</v>
-      </c>
-      <c r="O6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6" t="s">
-        <v>237</v>
-      </c>
-      <c r="S6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1839,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADCD556-2E3D-47E1-B933-FF703C658417}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -1904,21 +1713,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F2" t="s">
         <v>67</v>
@@ -1927,10 +1736,10 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
@@ -1942,7 +1751,7 @@
         <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -1950,30 +1759,28 @@
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2"/>
-      <c r="Q2"/>
       <c r="R2" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="S2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
         <v>67</v>
@@ -1982,10 +1789,10 @@
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="I3" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
@@ -1997,7 +1804,7 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="N3" t="s">
         <v>23</v>
@@ -2005,30 +1812,28 @@
       <c r="O3" t="s">
         <v>21</v>
       </c>
-      <c r="P3"/>
-      <c r="Q3"/>
       <c r="R3" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="S3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
         <v>67</v>
@@ -2037,22 +1842,22 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="I4" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="L4" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="M4" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="N4" t="s">
         <v>56</v>
@@ -2060,30 +1865,28 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4"/>
-      <c r="Q4"/>
       <c r="R4" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="S4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F5" t="s">
         <v>67</v>
@@ -2092,22 +1895,22 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="I5" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="L5" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="M5" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="N5" t="s">
         <v>56</v>
@@ -2115,10 +1918,8 @@
       <c r="O5" t="s">
         <v>21</v>
       </c>
-      <c r="P5"/>
-      <c r="Q5"/>
       <c r="R5" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="S5" t="s">
         <v>21</v>
@@ -2397,7 +2198,7 @@
         <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
         <v>83</v>
@@ -2409,34 +2210,34 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J5" t="s">
         <v>109</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>110</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>111</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>112</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>113</v>
-      </c>
-      <c r="N5" t="s">
-        <v>114</v>
       </c>
       <c r="O5" t="s">
         <v>56</v>
       </c>
       <c r="P5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q5" t="s">
         <v>85</v>
       </c>
       <c r="S5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T5" t="s">
         <v>73</v>
@@ -2445,7 +2246,7 @@
         <v>58</v>
       </c>
       <c r="V5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W5" t="s">
         <v>59</v>
@@ -2465,7 +2266,7 @@
         <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
         <v>83</v>
@@ -2486,25 +2287,25 @@
         <v>94</v>
       </c>
       <c r="L6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" t="s">
         <v>119</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>120</v>
-      </c>
-      <c r="N6" t="s">
-        <v>121</v>
       </c>
       <c r="O6" t="s">
         <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q6" t="s">
         <v>85</v>
       </c>
       <c r="S6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T6" t="s">
         <v>73</v>
@@ -2513,7 +2314,7 @@
         <v>58</v>
       </c>
       <c r="V6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W6" t="s">
         <v>59</v>
@@ -2530,10 +2331,10 @@
         <v>89</v>
       </c>
       <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
         <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>124</v>
       </c>
       <c r="E7" t="s">
         <v>83</v>
@@ -2545,34 +2346,34 @@
         <v>86</v>
       </c>
       <c r="I7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" t="s">
         <v>125</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>126</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>127</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>128</v>
       </c>
-      <c r="M7" t="s">
-        <v>129</v>
-      </c>
       <c r="N7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O7" t="s">
         <v>56</v>
       </c>
       <c r="P7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q7" t="s">
         <v>85</v>
       </c>
       <c r="S7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T7" t="s">
         <v>73</v>
@@ -2581,7 +2382,7 @@
         <v>58</v>
       </c>
       <c r="V7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W7" t="s">
         <v>59</v>
@@ -2598,10 +2399,10 @@
         <v>89</v>
       </c>
       <c r="C8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
         <v>131</v>
-      </c>
-      <c r="D8" t="s">
-        <v>132</v>
       </c>
       <c r="E8" t="s">
         <v>83</v>
@@ -2616,31 +2417,31 @@
         <v>93</v>
       </c>
       <c r="J8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" t="s">
         <v>133</v>
       </c>
-      <c r="K8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L8" t="s">
-        <v>134</v>
-      </c>
       <c r="M8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O8" t="s">
         <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q8" t="s">
         <v>85</v>
       </c>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T8" t="s">
         <v>73</v>
@@ -2649,7 +2450,7 @@
         <v>58</v>
       </c>
       <c r="V8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W8" t="s">
         <v>59</v>
@@ -2666,10 +2467,10 @@
         <v>89</v>
       </c>
       <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
         <v>136</v>
-      </c>
-      <c r="D9" t="s">
-        <v>137</v>
       </c>
       <c r="E9" t="s">
         <v>83</v>
@@ -2681,34 +2482,34 @@
         <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J9" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" t="s">
         <v>138</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>139</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>140</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>141</v>
-      </c>
-      <c r="N9" t="s">
-        <v>142</v>
       </c>
       <c r="O9" t="s">
         <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q9" t="s">
         <v>85</v>
       </c>
       <c r="S9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T9" t="s">
         <v>73</v>
@@ -2717,7 +2518,7 @@
         <v>58</v>
       </c>
       <c r="V9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W9" t="s">
         <v>59</v>
@@ -2737,7 +2538,7 @@
         <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
         <v>83</v>
@@ -2752,31 +2553,31 @@
         <v>93</v>
       </c>
       <c r="J10" t="s">
+        <v>146</v>
+      </c>
+      <c r="K10" t="s">
+        <v>138</v>
+      </c>
+      <c r="L10" t="s">
         <v>147</v>
       </c>
-      <c r="K10" t="s">
-        <v>139</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>148</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>149</v>
-      </c>
-      <c r="N10" t="s">
-        <v>150</v>
       </c>
       <c r="O10" t="s">
         <v>23</v>
       </c>
       <c r="P10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q10" t="s">
         <v>85</v>
       </c>
       <c r="S10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T10" t="s">
         <v>73</v>
@@ -2785,7 +2586,7 @@
         <v>58</v>
       </c>
       <c r="V10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W10" t="s">
         <v>59</v>
@@ -2802,46 +2603,46 @@
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
         <v>153</v>
-      </c>
-      <c r="F11" t="s">
-        <v>154</v>
       </c>
       <c r="H11" t="s">
         <v>92</v>
       </c>
       <c r="I11" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="J11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L11" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="M11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N11" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="O11" t="s">
         <v>56</v>
       </c>
       <c r="P11" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="S11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3092,7 +2893,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E73087-E198-4E54-9512-77DD5E310F31}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AL14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -3224,13 +3025,13 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
         <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
       </c>
       <c r="F2" t="s">
         <v>67</v>
@@ -3239,28 +3040,28 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="L2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="M2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="N2" t="s">
         <v>56</v>
       </c>
       <c r="R2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
@@ -3301,13 +3102,13 @@
         <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>154</v>
       </c>
       <c r="F3" t="s">
         <v>67</v>
@@ -3316,28 +3117,28 @@
         <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K3" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="L3" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="M3" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="N3" t="s">
         <v>56</v>
       </c>
       <c r="R3" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
@@ -3378,13 +3179,13 @@
         <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
         <v>153</v>
-      </c>
-      <c r="E4" t="s">
-        <v>154</v>
       </c>
       <c r="F4" t="s">
         <v>67</v>
@@ -3393,28 +3194,28 @@
         <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K4" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="L4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="M4" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="N4" t="s">
         <v>56</v>
       </c>
       <c r="R4" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S4" t="s">
         <v>21</v>
@@ -3455,13 +3256,13 @@
         <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="s">
         <v>153</v>
-      </c>
-      <c r="E5" t="s">
-        <v>154</v>
       </c>
       <c r="F5" t="s">
         <v>67</v>
@@ -3470,28 +3271,28 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K5" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="L5" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="N5" t="s">
         <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S5" t="s">
         <v>21</v>
@@ -3529,16 +3330,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" t="s">
         <v>152</v>
       </c>
-      <c r="C6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>153</v>
-      </c>
-      <c r="E6" t="s">
-        <v>154</v>
       </c>
       <c r="F6" t="s">
         <v>67</v>
@@ -3547,28 +3348,28 @@
         <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K6" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="L6" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="M6" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="N6" t="s">
         <v>56</v>
       </c>
       <c r="R6" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S6" t="s">
         <v>21</v>
@@ -3606,16 +3407,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
         <v>153</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
       </c>
       <c r="F7" t="s">
         <v>67</v>
@@ -3624,28 +3425,28 @@
         <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K7" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="L7" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="M7" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
       </c>
       <c r="R7" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S7" t="s">
         <v>21</v>
@@ -3683,16 +3484,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" t="s">
         <v>153</v>
-      </c>
-      <c r="E8" t="s">
-        <v>154</v>
       </c>
       <c r="F8" t="s">
         <v>67</v>
@@ -3701,28 +3502,28 @@
         <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K8" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="L8" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="M8" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="N8" t="s">
         <v>56</v>
       </c>
       <c r="R8" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S8" t="s">
         <v>21</v>
@@ -3760,16 +3561,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
         <v>153</v>
-      </c>
-      <c r="E9" t="s">
-        <v>154</v>
       </c>
       <c r="F9" t="s">
         <v>67</v>
@@ -3778,28 +3579,28 @@
         <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K9" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="L9" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="M9" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="N9" t="s">
         <v>56</v>
       </c>
       <c r="R9" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="S9" t="s">
         <v>21</v>
@@ -3837,16 +3638,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
         <v>153</v>
-      </c>
-      <c r="E10" t="s">
-        <v>154</v>
       </c>
       <c r="F10" t="s">
         <v>67</v>
@@ -3855,28 +3656,28 @@
         <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K10" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="L10" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="M10" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="N10" t="s">
         <v>56</v>
       </c>
       <c r="R10" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="S10" t="s">
         <v>21</v>
@@ -3909,8 +3710,364 @@
         <v>72</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K11" t="s">
+        <v>231</v>
+      </c>
+      <c r="L11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M11" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11" t="s">
+        <v>228</v>
+      </c>
+      <c r="S11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" t="s">
+        <v>155</v>
+      </c>
+      <c r="J12" t="s">
+        <v>236</v>
+      </c>
+      <c r="K12" t="s">
+        <v>237</v>
+      </c>
+      <c r="L12" t="s">
+        <v>238</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I13" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" t="s">
+        <v>236</v>
+      </c>
+      <c r="K13" t="s">
+        <v>241</v>
+      </c>
+      <c r="L13" t="s">
+        <v>242</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13" t="s">
+        <v>228</v>
+      </c>
+      <c r="S13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>196</v>
+      </c>
+      <c r="I14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" t="s">
+        <v>236</v>
+      </c>
+      <c r="K14" t="s">
+        <v>176</v>
+      </c>
+      <c r="L14" t="s">
+        <v>177</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14" t="s">
+        <v>228</v>
+      </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK14"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>